<commit_message>
fix nan in required data
</commit_message>
<xml_diff>
--- a/can_collect_redress_kits.xlsx
+++ b/can_collect_redress_kits.xlsx
@@ -494,7 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +563,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -595,26 +595,26 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>L107</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>Needle bearing, NK10/16</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>L107</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>Needle bearing, NK10/16</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -627,7 +627,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -659,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -691,7 +691,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="G7" s="1" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
@@ -755,7 +755,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0</v>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="G8" s="1" t="n">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>14</v>
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="G9" s="1" t="n">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>38</v>
@@ -819,7 +819,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0</v>
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="G10" s="1" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>12</v>
@@ -851,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0</v>
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="G11" s="1" t="n">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
@@ -899,7 +899,7 @@
         </is>
       </c>
       <c r="G12" s="1" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>4</v>
@@ -915,26 +915,698 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>R081</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>Retaining ring A6</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="inlineStr">
+        <is>
+          <t>R053</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>Retaining ring INCONEL X-750</t>
+        </is>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>R130</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>Retaining ring 218B</t>
+        </is>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>T135</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 48,00 x 1,20 - V80</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="inlineStr">
+        <is>
+          <t>RT21014</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>Screw M2,5x4 mm kval.12,9</t>
+        </is>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>T077</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>PTFE-Ring ø3,7/2,7x0,9</t>
+        </is>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="inlineStr">
+        <is>
+          <t>T081</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 30,0 x 1,0 - V70</t>
+        </is>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>T006</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 37,82 x 1,78 - V80</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>R023</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>Retaining ring</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>T095</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 3,00 x 1,00 - V70</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>T020</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 6,07 x 1,78 - V75</t>
+        </is>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0764</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>T049</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 14,00 x 1,78 - V75</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>T198</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>O-ring ø1,78 - V70 L=1423</t>
+        </is>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>T001</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 7,66 x 1,78 - V70</t>
+        </is>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>T070</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 4,50 x 1,00 - V70</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>T021</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 10,82 x 1,78 - V70</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>T071</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>Glide ring</t>
+        </is>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>KT22024</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>Screw M4</t>
+        </is>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>T006</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 37,82 x 1,78 - V70</t>
+        </is>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>T015</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 5,28 x 1,78-V70</t>
+        </is>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>T025</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 9,25 x 1,78 - V70</t>
+        </is>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>REDRESS0180</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>T020</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>O-ring 6,07 x 1,78 - V70</t>
+        </is>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>R081</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="inlineStr">
-        <is>
-          <t>Retaining ring A6</t>
-        </is>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -8826,7 +9498,7 @@
         </is>
       </c>
       <c r="B787" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="788">
@@ -9416,7 +10088,7 @@
         </is>
       </c>
       <c r="B846" t="n">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="847">
@@ -10046,7 +10718,7 @@
         </is>
       </c>
       <c r="B909" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="910">
@@ -10306,7 +10978,7 @@
         </is>
       </c>
       <c r="B935" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="936">
@@ -12496,7 +13168,7 @@
         </is>
       </c>
       <c r="B1154" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1155">
@@ -12606,7 +13278,7 @@
         </is>
       </c>
       <c r="B1165" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1166">
@@ -12646,7 +13318,7 @@
         </is>
       </c>
       <c r="B1169" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1170">
@@ -12806,7 +13478,7 @@
         </is>
       </c>
       <c r="B1185" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1186">
@@ -16106,7 +16778,7 @@
         </is>
       </c>
       <c r="B1515" t="n">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1516">
@@ -18686,7 +19358,7 @@
         </is>
       </c>
       <c r="B1773" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1774">
@@ -18776,7 +19448,7 @@
         </is>
       </c>
       <c r="B1782" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="1783">
@@ -18856,7 +19528,7 @@
         </is>
       </c>
       <c r="B1790" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1791">
@@ -18966,7 +19638,7 @@
         </is>
       </c>
       <c r="B1801" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="1802">
@@ -19066,7 +19738,7 @@
         </is>
       </c>
       <c r="B1811" t="n">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="1812">
@@ -19096,7 +19768,7 @@
         </is>
       </c>
       <c r="B1814" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="1815">
@@ -19146,7 +19818,7 @@
         </is>
       </c>
       <c r="B1819" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="1820">
@@ -19426,7 +20098,7 @@
         </is>
       </c>
       <c r="B1847" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="1848">
@@ -19656,7 +20328,7 @@
         </is>
       </c>
       <c r="B1870" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1871">
@@ -19666,7 +20338,7 @@
         </is>
       </c>
       <c r="B1871" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1872">
@@ -19706,7 +20378,7 @@
         </is>
       </c>
       <c r="B1875" t="n">
-        <v>355</v>
+        <v>323</v>
       </c>
     </row>
     <row r="1876">
@@ -19766,7 +20438,7 @@
         </is>
       </c>
       <c r="B1881" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1882">
@@ -19916,7 +20588,7 @@
         </is>
       </c>
       <c r="B1896" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1897">
@@ -20106,7 +20778,7 @@
         </is>
       </c>
       <c r="B1915" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1916">
@@ -20466,7 +21138,7 @@
         </is>
       </c>
       <c r="B1951" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1952">
@@ -21206,7 +21878,7 @@
         </is>
       </c>
       <c r="B2025" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2026">

</xml_diff>